<commit_message>
Edited the presentation and my slides a little
Issues my email address in the images for misp. Added a total row in the issues side.
</commit_message>
<xml_diff>
--- a/Class-Presentation/SWAMP Error Compilation.xlsx
+++ b/Class-Presentation/SWAMP Error Compilation.xlsx
@@ -107,9 +107,6 @@
     <t>JS</t>
   </si>
   <si>
-    <t>there must be a single space between the closing paranthasis and the opening brace of a multi-line IF statement found 0 spaces programming conventions</t>
-  </si>
-  <si>
     <t>the $_GET super global must not be accessed directly use SECURITY::getRequestData() instead</t>
   </si>
   <si>
@@ -134,15 +131,9 @@
     <t>File is being conditionally included, use "include" instead</t>
   </si>
   <si>
-    <t>closing paranthesis of a multi-line IF statement must be on a new line</t>
-  </si>
-  <si>
     <t>Arguments with default values must be at the end of the argument list</t>
   </si>
   <si>
-    <t>First condition of a multi-line IF statement must directly follow the opening paranthesis</t>
-  </si>
-  <si>
     <t>Empty ELSE statement detected</t>
   </si>
   <si>
@@ -164,18 +155,12 @@
     <t>scope not defined for 4 variables</t>
   </si>
   <si>
-    <t>using statements but including a set of parantheses when they are not needed</t>
-  </si>
-  <si>
     <t>joining strings using inline arrays is not allowed, use the '+' operator instead</t>
   </si>
   <si>
     <t>empty "For Each" statement detected</t>
   </si>
   <si>
-    <t>There must be a single space between the closing paranthasis and the opening brace of a multi-line IF statement found a new line</t>
-  </si>
-  <si>
     <t>abstract declaration must precede visibility declaration</t>
   </si>
   <si>
@@ -183,6 +168,21 @@
   </si>
   <si>
     <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>there must be a single space between the closing parenthesis and the opening brace of a multi-line IF statement found 0 spaces programming conventions</t>
+  </si>
+  <si>
+    <t>closing parenthesis of a multi-line IF statement must be on a new line</t>
+  </si>
+  <si>
+    <t>First condition of a multi-line IF statement must directly follow the opening parenthesis</t>
+  </si>
+  <si>
+    <t>using statements but including a set of parentheses when they are not needed</t>
+  </si>
+  <si>
+    <t>There must be a single space between the closing parenthesis and the opening brace of a multi-line IF statement found a new line</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -288,48 +288,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -353,7 +355,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -373,13 +381,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D39"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Software" dataDxfId="5"/>
-    <tableColumn id="2" name="Count" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" name="Software" dataDxfId="3"/>
+    <tableColumn id="2" name="Count" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,7 +893,7 @@
         <v>124</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -896,7 +904,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -907,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -918,7 +926,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -929,7 +937,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -940,7 +948,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -951,7 +959,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -962,7 +970,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -973,7 +981,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -984,7 +992,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -995,7 +1003,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -1006,7 +1014,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1017,7 +1025,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1028,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -1039,7 +1047,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1050,7 +1058,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1061,7 +1069,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1072,7 +1080,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1083,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1094,7 +1102,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1105,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1116,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="58" x14ac:dyDescent="0.35">
@@ -1127,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1138,12 +1146,12 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2">
         <f>SUM(B2:B39)</f>
@@ -1159,6 +1167,10 @@
         <f>SUM(B2,B4,B5,B6,B7,B8,B10,B12,B13,B17,B18,B24)</f>
         <v>17568</v>
       </c>
+      <c r="C42" s="9">
+        <f>B42/$B$40</f>
+        <v>0.79110190480479126</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
@@ -1168,6 +1180,10 @@
         <f>SUM(B3,B11,B14,B15,B19,B20,B21,B22,B23,B25,B26,B27,B28,B29,B30,B31,B32,B33,B34,B35,B36,B37,B38,B39)</f>
         <v>3955</v>
       </c>
+      <c r="C43" s="9">
+        <f t="shared" ref="C43:C45" si="0">B43/$B$40</f>
+        <v>0.17809699644256316</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
@@ -1177,6 +1193,10 @@
         <f>SUM(B9)</f>
         <v>560</v>
       </c>
+      <c r="C44" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5217273832575313E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
@@ -1186,14 +1206,22 @@
         <f>SUM(B16)</f>
         <v>124</v>
       </c>
+      <c r="C45" s="9">
+        <f t="shared" si="0"/>
+        <v>5.5838249200702485E-3</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2">
         <f>SUM(B42:B45)</f>
         <v>22207</v>
+      </c>
+      <c r="C47" s="10">
+        <f>SUM(C42:C45)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>